<commit_message>
update size of takeABreakProgress
</commit_message>
<xml_diff>
--- a/examples/tables/testTakeABreak.xlsx
+++ b/examples/tables/testTakeABreak.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/denispelli/Dropbox/EasyEyes/Experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18765AE2-7969-E74D-8F86-E098B76F227F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C970D53-9040-0B48-BB2A-ADEF1E9FE942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="500" windowWidth="24840" windowHeight="13420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
   <si>
     <t>_about</t>
   </si>
@@ -131,6 +131,12 @@
   </si>
   <si>
     <t xml:space="preserve"> Take a break after every other trial.</t>
+  </si>
+  <si>
+    <t>responseTypedBool</t>
+  </si>
+  <si>
+    <t>takeABreakMinimumDurationSec</t>
   </si>
 </sst>
 </file>
@@ -971,10 +977,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1055,15 +1061,15 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="B8" t="b">
         <v>1</v>
@@ -1074,210 +1080,232 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="B10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>10</v>
+        <v>35</v>
+      </c>
+      <c r="B11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13">
-        <v>0.5</v>
-      </c>
-      <c r="C13">
-        <v>0.5</v>
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" t="s">
-        <v>32</v>
+        <v>38</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="B15">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="C15">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16">
-        <v>-10</v>
-      </c>
-      <c r="C16">
-        <v>10</v>
+        <v>34</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" t="s">
-        <v>17</v>
+        <v>14</v>
+      </c>
+      <c r="B18">
+        <v>-10</v>
+      </c>
+      <c r="C18">
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" t="s">
-        <v>19</v>
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20">
-        <v>8</v>
-      </c>
-      <c r="C20">
-        <v>8</v>
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>2.2999999999999998</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>2.2999999999999998</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23">
-        <v>0.01</v>
-      </c>
-      <c r="C23">
-        <v>0.01</v>
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B24">
-        <v>2</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="C24">
-        <v>2</v>
+        <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B25">
-        <v>3</v>
+        <v>0.01</v>
       </c>
       <c r="C25">
-        <v>3</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" t="s">
-        <v>28</v>
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>29</v>
       </c>
-      <c r="B27">
+      <c r="B29">
         <v>50</v>
       </c>
-      <c r="C27">
+      <c r="C29">
         <v>50</v>
       </c>
     </row>

</xml_diff>